<commit_message>
Correções na tabela-verdade e slides do multiciclo
</commit_message>
<xml_diff>
--- a/Laboratorio_3/Tabela-verdade_Controle_RISCV.xlsx
+++ b/Laboratorio_3/Tabela-verdade_Controle_RISCV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luthiery\Desktop\Quartus_files\OAC\TrabalhosOAC\Laboratorio_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4045F417-3AE1-4E39-9869-809FD1A5AA8A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{75880AC9-D06A-494E-9A36-4D21A20902E0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="116">
   <si>
     <t>Instrução</t>
   </si>
@@ -800,6 +800,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -807,15 +816,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1203,7 +1203,7 @@
   <dimension ref="A1:AMH48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1918,8 +1918,8 @@
       <c r="K17" s="5">
         <v>0</v>
       </c>
-      <c r="L17" s="31" t="s">
-        <v>15</v>
+      <c r="L17" s="31">
+        <v>0</v>
       </c>
       <c r="N17" s="2">
         <v>1</v>
@@ -2474,8 +2474,8 @@
       <c r="K31" s="5">
         <v>0</v>
       </c>
-      <c r="L31" s="30">
-        <v>1</v>
+      <c r="L31" s="30" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="16.350000000000001" customHeight="1">
@@ -2774,8 +2774,8 @@
       <c r="K39" s="36">
         <v>11</v>
       </c>
-      <c r="L39" s="38" t="s">
-        <v>15</v>
+      <c r="L39" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="16.350000000000001" customHeight="1">
@@ -3113,7 +3113,7 @@
   <dimension ref="A1:AMB1048574"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4112,16 +4112,16 @@
       <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="78">
-        <v>1</v>
-      </c>
-      <c r="D2" s="78">
+      <c r="C2" s="75">
+        <v>1</v>
+      </c>
+      <c r="D2" s="75">
         <v>0</v>
       </c>
       <c r="E2" s="2">
@@ -4139,10 +4139,10 @@
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A3" s="76"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -4160,16 +4160,16 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="75">
-        <v>1</v>
-      </c>
-      <c r="D4" s="75">
+      <c r="C4" s="78">
+        <v>1</v>
+      </c>
+      <c r="D4" s="78">
         <v>1</v>
       </c>
       <c r="E4" s="2">
@@ -4189,10 +4189,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A5" s="73"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
       <c r="E5" s="2">
         <v>1</v>
       </c>
@@ -4210,19 +4210,19 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="75">
-        <v>1</v>
-      </c>
-      <c r="D6" s="75">
+      <c r="C6" s="78">
+        <v>1</v>
+      </c>
+      <c r="D6" s="78">
         <v>100</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="77" t="s">
         <v>102</v>
       </c>
       <c r="F6" s="53" t="s">
@@ -4239,11 +4239,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A7" s="73"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="74"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="53" t="s">
         <v>110</v>
       </c>
@@ -4253,19 +4253,19 @@
       <c r="I7" s="62"/>
     </row>
     <row r="8" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="75">
-        <v>1</v>
-      </c>
-      <c r="D8" s="75">
+      <c r="C8" s="78">
+        <v>1</v>
+      </c>
+      <c r="D8" s="78">
         <v>101</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="77" t="s">
         <v>102</v>
       </c>
       <c r="F8" s="53" t="s">
@@ -4277,11 +4277,11 @@
       <c r="I8" s="62"/>
     </row>
     <row r="9" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A9" s="73"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="74"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="53" t="s">
         <v>110</v>
       </c>
@@ -4291,19 +4291,19 @@
       <c r="I9" s="62"/>
     </row>
     <row r="10" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="75">
-        <v>1</v>
-      </c>
-      <c r="D10" s="75">
+      <c r="C10" s="78">
+        <v>1</v>
+      </c>
+      <c r="D10" s="78">
         <v>110</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="77" t="s">
         <v>102</v>
       </c>
       <c r="F10" s="53" t="s">
@@ -4315,11 +4315,11 @@
       <c r="I10" s="62"/>
     </row>
     <row r="11" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A11" s="73"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="74"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="77"/>
       <c r="F11" s="53" t="s">
         <v>110</v>
       </c>
@@ -4329,19 +4329,19 @@
       <c r="I11" s="62"/>
     </row>
     <row r="12" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="75">
-        <v>1</v>
-      </c>
-      <c r="D12" s="75">
+      <c r="C12" s="78">
+        <v>1</v>
+      </c>
+      <c r="D12" s="78">
         <v>111</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="77" t="s">
         <v>102</v>
       </c>
       <c r="F12" s="53" t="s">
@@ -4353,11 +4353,11 @@
       <c r="I12" s="62"/>
     </row>
     <row r="13" spans="1:10" ht="16.350000000000001" customHeight="1">
-      <c r="A13" s="73"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="74"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="77"/>
       <c r="F13" s="53" t="s">
         <v>110</v>
       </c>
@@ -4440,6 +4440,26 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -4448,26 +4468,6 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>